<commit_message>
Add of 4 skills
</commit_message>
<xml_diff>
--- a/Skills.xlsx
+++ b/Skills.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,14 +9,159 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Vie</t>
+  </si>
+  <si>
+    <t>Stats Requises</t>
+  </si>
+  <si>
+    <t>Effet</t>
+  </si>
+  <si>
+    <t>Coût Stamina</t>
+  </si>
+  <si>
+    <t>Coût vie</t>
+  </si>
+  <si>
+    <t>Passif / Actif</t>
+  </si>
+  <si>
+    <t>Vitalité</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Skill Requis</t>
+  </si>
+  <si>
+    <t>Robustesse</t>
+  </si>
+  <si>
+    <t>Position Défensive</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Cible (L, A, E, T)</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Position (CaC, P, T)</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 Robustesse</t>
+  </si>
+  <si>
+    <t>30 Vie</t>
+  </si>
+  <si>
+    <t>Fatigue</t>
+  </si>
+  <si>
+    <t>Effort</t>
+  </si>
+  <si>
+    <t>2 Stamina</t>
+  </si>
+  <si>
+    <t>Attaque Physique</t>
+  </si>
+  <si>
+    <t>Frappe Concentrée</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>CaC</t>
+  </si>
+  <si>
+    <t>150% Attaque Physique</t>
+  </si>
+  <si>
+    <t>Attaque Magique</t>
+  </si>
+  <si>
+    <t>Esquive</t>
+  </si>
+  <si>
+    <t>Tir Energetique</t>
+  </si>
+  <si>
+    <t>150% Attaque Magique</t>
+  </si>
+  <si>
+    <t>Instinct</t>
+  </si>
+  <si>
+    <t>3% Esquive</t>
+  </si>
+  <si>
+    <t>170% AttaqueMagique</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>50% Attaque Magique</t>
+  </si>
+  <si>
+    <t>Tir Elementaire</t>
+  </si>
+  <si>
+    <t>Tir de glace</t>
+  </si>
+  <si>
+    <t>Orbe Revigorante</t>
+  </si>
+  <si>
+    <t>Boule de Feu</t>
+  </si>
+  <si>
+    <t>150% Attaque Magique  
+(-) 5% Esquive</t>
+  </si>
+  <si>
+    <t>170% Attaque Magique  
+30% de chance :  
+- 15% Attaque Magique | 2 tours</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +177,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -40,23 +185,238 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +493,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +701,783 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="17" customWidth="1"/>
+    <col min="2" max="3" width="26" style="17" customWidth="1"/>
+    <col min="4" max="4" width="24" style="17" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="30" style="17" customWidth="1"/>
+    <col min="8" max="8" width="13" style="17" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="12">
+        <v>5</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
+        <v>1</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+      <c r="I32" s="13">
+        <v>1</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="12">
+        <v>10</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0</v>
+      </c>
+      <c r="I33" s="13">
+        <v>2</v>
+      </c>
+      <c r="J33" s="12" t="str">
+        <f>B32</f>
+        <v>Tir Energetique</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="12">
+        <v>10</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0</v>
+      </c>
+      <c r="I34" s="13">
+        <v>2</v>
+      </c>
+      <c r="J34" s="12" t="str">
+        <f>B32</f>
+        <v>Tir Energetique</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="12">
+        <v>20</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0</v>
+      </c>
+      <c r="I35" s="13">
+        <v>3</v>
+      </c>
+      <c r="J35" s="12" t="str">
+        <f>B33</f>
+        <v>Tir Elementaire</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="12">
+        <v>20</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0</v>
+      </c>
+      <c r="I36" s="13">
+        <v>3</v>
+      </c>
+      <c r="J36" s="12" t="str">
+        <f>B33</f>
+        <v>Tir Elementaire</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0</v>
+      </c>
+      <c r="I39" s="13">
+        <v>0</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add of racial passive skills
</commit_message>
<xml_diff>
--- a/Skills.xlsx
+++ b/Skills.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
   <si>
     <t>Nom</t>
   </si>
@@ -254,6 +254,45 @@
   </si>
   <si>
     <t>Infatiguable</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Nain</t>
+  </si>
+  <si>
+    <t>Humain</t>
+  </si>
+  <si>
+    <t>Geant</t>
+  </si>
+  <si>
+    <t>Avarie</t>
+  </si>
+  <si>
+    <t>Negocieur</t>
+  </si>
+  <si>
+    <t>Elfe</t>
+  </si>
+  <si>
+    <t>Transporteur</t>
+  </si>
+  <si>
+    <t>5% de gold en plus</t>
+  </si>
+  <si>
+    <t>5% de bonus chez les marchands</t>
+  </si>
+  <si>
+    <t>30 kg en plus dans l'inventaire</t>
+  </si>
+  <si>
+    <t>Je sais pas</t>
+  </si>
+  <si>
+    <t>Truc d'elfe</t>
   </si>
 </sst>
 </file>
@@ -563,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -601,13 +640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -644,6 +677,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -950,24 +986,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="16" customWidth="1"/>
-    <col min="2" max="3" width="26" style="16" customWidth="1"/>
-    <col min="4" max="4" width="24" style="16" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="30" style="16" customWidth="1"/>
-    <col min="8" max="8" width="13" style="16" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="14" customWidth="1"/>
+    <col min="2" max="3" width="26" style="14" customWidth="1"/>
+    <col min="4" max="4" width="24" style="14" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="30" style="14" customWidth="1"/>
+    <col min="8" max="8" width="13" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1028,12 +1064,12 @@
       <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="21" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="10" t="s">
         <v>55</v>
       </c>
@@ -1058,13 +1094,13 @@
       <c r="I3" s="12">
         <v>3</v>
       </c>
-      <c r="J3" s="24" t="str">
+      <c r="J3" s="22" t="str">
         <f>B2</f>
         <v>Vitalité</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="10" t="s">
         <v>66</v>
       </c>
@@ -1089,13 +1125,13 @@
       <c r="I4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="24" t="str">
+      <c r="J4" s="22" t="str">
         <f>B2</f>
         <v>Vitalité</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="10" t="s">
         <v>67</v>
       </c>
@@ -1120,13 +1156,13 @@
       <c r="I5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="24" t="str">
+      <c r="J5" s="22" t="str">
         <f>B4</f>
         <v>Vitalité 2</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="10" t="s">
         <v>70</v>
       </c>
@@ -1151,13 +1187,13 @@
       <c r="I6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="24" t="str">
+      <c r="J6" s="22" t="str">
         <f>B5</f>
         <v>Vitalité 3</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="10" t="s">
         <v>68</v>
       </c>
@@ -1182,25 +1218,25 @@
       <c r="I7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="24" t="str">
+      <c r="J7" s="22" t="str">
         <f>B6</f>
         <v>Vitalité d'Ogre</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1227,12 +1263,12 @@
       <c r="I9" s="9">
         <v>1</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="10" t="s">
         <v>50</v>
       </c>
@@ -1257,13 +1293,13 @@
       <c r="I10" s="12">
         <v>3</v>
       </c>
-      <c r="J10" s="24" t="str">
+      <c r="J10" s="22" t="str">
         <f>B9</f>
         <v>Position Défensive</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
@@ -1288,13 +1324,13 @@
       <c r="I11" s="12">
         <v>2</v>
       </c>
-      <c r="J11" s="24" t="str">
+      <c r="J11" s="22" t="str">
         <f>B9</f>
         <v>Position Défensive</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="10" t="s">
         <v>53</v>
       </c>
@@ -1319,13 +1355,13 @@
       <c r="I12" s="12">
         <v>4</v>
       </c>
-      <c r="J12" s="24" t="str">
+      <c r="J12" s="22" t="str">
         <f>B11</f>
         <v>Bouclier Magique</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1334,10 +1370,10 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="12"/>
-      <c r="J13" s="24"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -1346,22 +1382,22 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="24"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1388,12 +1424,12 @@
       <c r="I16" s="9">
         <v>0</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
@@ -1418,13 +1454,13 @@
       <c r="I17" s="9">
         <v>0</v>
       </c>
-      <c r="J17" s="25" t="str">
+      <c r="J17" s="23" t="str">
         <f>B16</f>
         <v>Infatiguable</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1433,10 +1469,10 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="12"/>
-      <c r="J18" s="24"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -1445,22 +1481,22 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="12"/>
-      <c r="J19" s="24"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1487,12 +1523,12 @@
       <c r="I21" s="9">
         <v>1</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1517,13 +1553,13 @@
       <c r="I22" s="9">
         <v>3</v>
       </c>
-      <c r="J22" s="25" t="str">
+      <c r="J22" s="23" t="str">
         <f>B21</f>
         <v>Frappe Concentrée</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="10" t="s">
         <v>48</v>
       </c>
@@ -1542,19 +1578,19 @@
       <c r="G23" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="24">
         <v>0.1</v>
       </c>
       <c r="I23" s="12">
         <v>2</v>
       </c>
-      <c r="J23" s="24" t="str">
+      <c r="J23" s="22" t="str">
         <f>B21</f>
         <v>Frappe Concentrée</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="10" t="s">
         <v>61</v>
       </c>
@@ -1579,13 +1615,13 @@
       <c r="I24" s="12">
         <v>3</v>
       </c>
-      <c r="J24" s="24" t="str">
+      <c r="J24" s="22" t="str">
         <f>B22</f>
         <v>Coup déstabilisant</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="10" t="s">
         <v>64</v>
       </c>
@@ -1608,10 +1644,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="12"/>
-      <c r="J25" s="24"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -1620,22 +1656,22 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="12"/>
-      <c r="J26" s="24"/>
+      <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="18"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -1662,12 +1698,12 @@
       <c r="I28" s="9">
         <v>1</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="10" t="s">
         <v>34</v>
       </c>
@@ -1692,13 +1728,13 @@
       <c r="I29" s="12">
         <v>2</v>
       </c>
-      <c r="J29" s="24" t="str">
+      <c r="J29" s="22" t="str">
         <f>B28</f>
         <v>Tir Energetique</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="10" t="s">
         <v>36</v>
       </c>
@@ -1723,13 +1759,13 @@
       <c r="I30" s="12">
         <v>2</v>
       </c>
-      <c r="J30" s="24" t="str">
+      <c r="J30" s="22" t="str">
         <f>B28</f>
         <v>Tir Energetique</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="10" t="s">
         <v>35</v>
       </c>
@@ -1754,13 +1790,13 @@
       <c r="I31" s="12">
         <v>3</v>
       </c>
-      <c r="J31" s="24" t="str">
+      <c r="J31" s="22" t="str">
         <f>B29</f>
         <v>Tir Elementaire</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="10" t="s">
         <v>37</v>
       </c>
@@ -1785,13 +1821,13 @@
       <c r="I32" s="12">
         <v>3</v>
       </c>
-      <c r="J32" s="24" t="str">
+      <c r="J32" s="22" t="str">
         <f>B29</f>
         <v>Tir Elementaire</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="10" t="s">
         <v>41</v>
       </c>
@@ -1816,13 +1852,13 @@
       <c r="I33" s="12">
         <v>3</v>
       </c>
-      <c r="J33" s="24" t="str">
+      <c r="J33" s="22" t="str">
         <f>B30</f>
         <v>Orbe Revigorante</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="10" t="s">
         <v>59</v>
       </c>
@@ -1847,13 +1883,13 @@
       <c r="I34" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J34" s="24" t="str">
+      <c r="J34" s="22" t="str">
         <f>B32</f>
         <v>Boule de Feu</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -1862,10 +1898,10 @@
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="12"/>
-      <c r="J35" s="24"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -1874,10 +1910,10 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="24"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -1886,22 +1922,22 @@
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="12"/>
-      <c r="J37" s="24"/>
+      <c r="J37" s="22"/>
     </row>
     <row r="38" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1928,12 +1964,12 @@
       <c r="I39" s="9">
         <v>0</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="J39" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="10" t="s">
         <v>44</v>
       </c>
@@ -1958,13 +1994,13 @@
       <c r="I40" s="12">
         <v>3</v>
       </c>
-      <c r="J40" s="24" t="str">
+      <c r="J40" s="22" t="str">
         <f>B39</f>
         <v>Instinct</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19"/>
       <c r="B41" s="10" t="s">
         <v>46</v>
       </c>
@@ -1989,13 +2025,13 @@
       <c r="I41" s="12">
         <v>4</v>
       </c>
-      <c r="J41" s="24" t="str">
+      <c r="J41" s="22" t="str">
         <f>B39</f>
         <v>Instinct</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="26"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
@@ -2003,11 +2039,11 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="24"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="22"/>
     </row>
     <row r="43" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
@@ -2015,32 +2051,162 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="24"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="18"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
+    <row r="45" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="23"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add of elves passive skill
</commit_message>
<xml_diff>
--- a/Skills.xlsx
+++ b/Skills.xlsx
@@ -289,10 +289,10 @@
     <t>30 kg en plus dans l'inventaire</t>
   </si>
   <si>
-    <t>Je sais pas</t>
-  </si>
-  <si>
-    <t>Truc d'elfe</t>
+    <t>Constitution régénérente</t>
+  </si>
+  <si>
+    <t>Soin entre les zones</t>
   </si>
 </sst>
 </file>
@@ -316,15 +316,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -598,11 +604,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -681,6 +743,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,11 +1063,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,45 +2147,45 @@
       <c r="A45" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="23"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="11" t="s">
+      <c r="D46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J46" s="22" t="s">
+      <c r="H46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="23" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2176,37 +2253,40 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J49" s="22" t="s">
-        <v>9</v>
-      </c>
+      <c r="H49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G51" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>